<commit_message>
Version from 2011-09-03. Updated TR
</commit_message>
<xml_diff>
--- a/media/papers/TR/CollisionsWithAndWithoutFrequencies.xlsx
+++ b/media/papers/TR/CollisionsWithAndWithoutFrequencies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1-1" sheetId="1" r:id="rId1"/>
@@ -1338,11 +1338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="232768256"/>
-        <c:axId val="232769792"/>
+        <c:axId val="124190720"/>
+        <c:axId val="124192256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="232768256"/>
+        <c:axId val="124190720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1352,12 +1352,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232769792"/>
+        <c:crossAx val="124192256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232769792"/>
+        <c:axId val="124192256"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1369,7 +1369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232768256"/>
+        <c:crossAx val="124190720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2627,11 +2627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233421824"/>
-        <c:axId val="233423616"/>
+        <c:axId val="124209408"/>
+        <c:axId val="124223488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233421824"/>
+        <c:axId val="124209408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2640,12 +2640,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233423616"/>
+        <c:crossAx val="124223488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233423616"/>
+        <c:axId val="124223488"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2657,7 +2657,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233421824"/>
+        <c:crossAx val="124209408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3915,11 +3915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233465344"/>
-        <c:axId val="233466880"/>
+        <c:axId val="124093184"/>
+        <c:axId val="124094720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233465344"/>
+        <c:axId val="124093184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3928,12 +3928,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233466880"/>
+        <c:crossAx val="124094720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233466880"/>
+        <c:axId val="124094720"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3945,7 +3945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233465344"/>
+        <c:crossAx val="124093184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3983,7 +3983,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.3864974831209986E-2"/>
+          <c:y val="3.2167230725885468E-2"/>
+          <c:w val="0.91346261639068271"/>
+          <c:h val="0.89525083810416783"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3991,15 +4001,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-8'!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>FQ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Frequencies Based Conflict Resolution</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -4595,15 +4597,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'1-8'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Simplified Conflict Resolution</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -5203,25 +5197,56 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="232662528"/>
-        <c:axId val="232664064"/>
+        <c:axId val="123929344"/>
+        <c:axId val="123930880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="232662528"/>
+        <c:axId val="123929344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Experiments ranked by the number of collisions in simplified</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:t> approach</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.22574614939755738"/>
+              <c:y val="0.85743868066035411"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232664064"/>
+        <c:crossAx val="123930880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232664064"/>
+        <c:axId val="123930880"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -5229,19 +5254,65 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Collisions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.5627987831377665E-2"/>
+              <c:y val="0.40906258947097063"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232662528"/>
+        <c:crossAx val="123929344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11125597566275533"/>
+          <c:y val="5.6474133692871173E-2"/>
+          <c:w val="0.38103405913895705"/>
+          <c:h val="0.14824229109562087"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6494,11 +6565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46556288"/>
-        <c:axId val="46503040"/>
+        <c:axId val="123980800"/>
+        <c:axId val="124011264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46556288"/>
+        <c:axId val="123980800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -6508,12 +6579,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46503040"/>
+        <c:crossAx val="124011264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46503040"/>
+        <c:axId val="124011264"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -6525,7 +6596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46556288"/>
+        <c:crossAx val="123980800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15715,8 +15786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U313"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21309,7 +21380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>

</xml_diff>